<commit_message>
Updated V1 QC Incident Cases Rules
</commit_message>
<xml_diff>
--- a/BCRPP_QC_R_Excel_Program/BCRPP_QC_DataDictionary_Version_1/Incident Cases Rules/BCRPP Incident Cases Warning Rules.xlsx
+++ b/BCRPP_QC_R_Excel_Program/BCRPP_QC_DataDictionary_Version_1/Incident Cases Rules/BCRPP Incident Cases Warning Rules.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28116"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0B1D6D-2F36-4873-9AD2-0FDE7681B1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{924638A6-C5CE-584C-922A-A1365CBB5852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52B81FA3-43DA-47CD-8B12-DBDB7A318026}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38200" yWindow="-1200" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="101">
   <si>
     <t>Variable</t>
   </si>
@@ -95,6 +95,24 @@
     <t>Comments</t>
   </si>
   <si>
+    <t>lastfup</t>
+  </si>
+  <si>
+    <t>crossrange.warnings</t>
+  </si>
+  <si>
+    <t>dxdate_primary1</t>
+  </si>
+  <si>
+    <t>dxdate_primary1 &lt;= lastfup| lastfup==8888</t>
+  </si>
+  <si>
+    <t>!lastfup %in% c(7777,8888)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">please confirm lastfup is before dxdate_primary1 </t>
+  </si>
+  <si>
     <t>detection_primary1</t>
   </si>
   <si>
@@ -119,9 +137,6 @@
     <t>crossvalid1.warnings</t>
   </si>
   <si>
-    <t>crossrange.warnings</t>
-  </si>
-  <si>
     <t>detection_detail_primary1 should be 888 when detection_primary1 is 888</t>
   </si>
   <si>
@@ -194,6 +209,9 @@
     <t>size_primary1 should be between 20 and 50 mm when sizecat_primary1 is 2</t>
   </si>
   <si>
+    <t>size_primary1 &gt;= 50 | size_primary1  == 888</t>
+  </si>
+  <si>
     <t>size_primary1 should be greater than 50 mm when sizecat_primary1 is 3</t>
   </si>
   <si>
@@ -275,6 +293,9 @@
     <t>size_primary2 should be between 20 and 50 mm when sizecat_primary2 is 2</t>
   </si>
   <si>
+    <t>size_primary2 &gt;= 50 | size_primary2  == 888</t>
+  </si>
+  <si>
     <t>size_primary2 should be greater than 50 mm when sizecat_primary2 is 3</t>
   </si>
   <si>
@@ -315,19 +336,13 @@
   </si>
   <si>
     <t>ki67cat_primary2 does not have recognized values</t>
-  </si>
-  <si>
-    <t>size_primary1 &gt; 50 &amp; size_primary1 &lt;= 100 | size_primary1  == 888</t>
-  </si>
-  <si>
-    <t>size_primary2 &gt; 50 &amp; size_primary2 &lt;= 100 | size_primary2  == 888</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +372,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -378,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -389,6 +410,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,37 +715,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T33"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="72.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="83.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="74.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="87.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="18.95">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,49 +807,55 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:20" s="2" customFormat="1" ht="18.75">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="37" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="J2" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="18.95">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -842,34 +870,30 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="3" t="s">
-        <v>24</v>
+      <c r="S3" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="37" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="39.950000000000003">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2">
-        <v>888</v>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="2">
-        <v>888</v>
-      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -878,30 +902,34 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="4" t="s">
-        <v>24</v>
+      <c r="S4" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="39.950000000000003">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
+      <c r="E5" s="2">
+        <v>888</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="I5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="2">
+        <v>888</v>
+      </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -910,24 +938,24 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="5" t="s">
+      <c r="S5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="18.95">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -942,24 +970,24 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-      <c r="S6" s="2" t="s">
-        <v>32</v>
+      <c r="S6" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="37" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="18.95">
+      <c r="A7" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -974,34 +1002,30 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="3" t="s">
-        <v>34</v>
+      <c r="S7" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="37" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="39.950000000000003">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>888</v>
+      <c r="E8" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="2">
-        <v>888</v>
-      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1010,30 +1034,34 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="4" t="s">
-        <v>34</v>
+      <c r="S8" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="39.950000000000003">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>38</v>
+      <c r="E9" s="2">
+        <v>888</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="I9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="2">
+        <v>888</v>
+      </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -1042,24 +1070,24 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="5" t="s">
-        <v>37</v>
+      <c r="S9" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="18.95">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1074,24 +1102,24 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="4" t="s">
-        <v>40</v>
+      <c r="S10" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="20.100000000000001">
       <c r="A11" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1106,24 +1134,24 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="2" t="s">
-        <v>43</v>
+      <c r="S11" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="18.95">
       <c r="A12" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1138,36 +1166,30 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-      <c r="S12" s="5" t="s">
-        <v>46</v>
+      <c r="S12" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="18.95">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13" s="2">
-        <v>1</v>
-      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -1176,35 +1198,35 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="2" t="s">
-        <v>48</v>
+      <c r="S13" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="18.95">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="J14" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -1215,34 +1237,34 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="5" t="s">
-        <v>46</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="18.95">
+      <c r="A15" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="J15" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -1253,32 +1275,34 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="T15" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
-        <v>46</v>
+      <c r="T15" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="18.95">
+      <c r="A16" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2">
-        <v>888</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="I16" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="J16" s="2">
-        <v>888</v>
+        <v>3</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -1289,29 +1313,33 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="18.95">
       <c r="A17" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2" t="s">
-        <v>56</v>
+      <c r="E17" s="2">
+        <v>888</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" s="2">
+        <v>888</v>
+      </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -1321,23 +1349,23 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="18.95">
       <c r="A18" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1353,23 +1381,23 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="18.95">
       <c r="A19" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1384,36 +1412,30 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
-      <c r="S19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="T19" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="S19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="18.95">
       <c r="A20" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -1423,29 +1445,35 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
       <c r="S20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="T20" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+      <c r="T20" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="18.95">
       <c r="A21" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="G21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -1455,23 +1483,23 @@
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="T21" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="T21" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="18.95">
       <c r="A22" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1486,24 +1514,24 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
-      <c r="S22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="S22" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="T22" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="20.100000000000001">
       <c r="A23" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1518,24 +1546,24 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
-      <c r="S23" s="2" t="s">
-        <v>71</v>
+      <c r="S23" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="18.95">
       <c r="A24" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1550,36 +1578,30 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="5" t="s">
-        <v>73</v>
+      <c r="S24" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="18.95">
       <c r="A25" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F25" s="2"/>
-      <c r="G25" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J25" s="2">
-        <v>1</v>
-      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -1588,35 +1610,35 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
-      <c r="S25" s="2" t="s">
-        <v>75</v>
+      <c r="S25" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="18.95">
       <c r="A26" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="J26" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -1627,34 +1649,34 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="S26" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="T26" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="18.95">
+      <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A27" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="B27" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="J27" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -1665,32 +1687,34 @@
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="T27" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>81</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="18.95">
       <c r="A28" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="2">
-        <v>888</v>
-      </c>
+      <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="I28" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="J28" s="2">
-        <v>888</v>
+        <v>3</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -1701,87 +1725,91 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="T28" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="T28" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="18.95">
       <c r="A29" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="T29" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>79</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2">
+        <v>888</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J29" s="2">
+        <v>888</v>
+      </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="18.95">
       <c r="A30" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="T30" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>89</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="T30" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" ht="18.95">
       <c r="A31" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -1797,35 +1825,29 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="T31" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" ht="18.95">
       <c r="A32" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="F32" s="2"/>
-      <c r="G32" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>90</v>
-      </c>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
@@ -1834,30 +1856,36 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
-      <c r="S32" s="5" t="s">
-        <v>88</v>
+      <c r="S32" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="18.95">
       <c r="A33" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
+      <c r="G33" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
@@ -1867,10 +1895,42 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="18.95">
+      <c r="A34" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1885,7 +1945,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1898,7 +1958,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>